<commit_message>
Mise à jour site Bois
</commit_message>
<xml_diff>
--- a/prix/prix.xlsx
+++ b/prix/prix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bois\prix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bois\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBCDB76-0C63-4C50-AE18-9C8CAD8F0B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578EBAA7-0E11-42C3-BDCF-6F2F88C3BB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="19416" windowHeight="11016" xr2:uid="{6E95DC93-531D-460D-9A06-44397A8920D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E95DC93-531D-460D-9A06-44397A8920D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="461">
   <si>
     <t>path</t>
   </si>
@@ -1371,6 +1371,54 @@
   </si>
   <si>
     <t>31099106</t>
+  </si>
+  <si>
+    <t>galerie/toupret-enduit-rebouchage-pate.png</t>
+  </si>
+  <si>
+    <t>galerie/toupret-wood-finish.png</t>
+  </si>
+  <si>
+    <t>galerie/toupret-hard-wood.png</t>
+  </si>
+  <si>
+    <t>galerie/toupret-repar-wood.png</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-blanc.jpg</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-chene-clair.jpg</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-chene-fonce.jpg</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-chene-moyen.jpg</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-naturel.jpg</t>
+  </si>
+  <si>
+    <t>galerie/pate-a-bois-50g-noyer.jpg</t>
+  </si>
+  <si>
+    <t>330ml</t>
+  </si>
+  <si>
+    <t>400g</t>
+  </si>
+  <si>
+    <t>1kg</t>
+  </si>
+  <si>
+    <t>80ml</t>
+  </si>
+  <si>
+    <t>1l</t>
+  </si>
+  <si>
+    <t>50g</t>
   </si>
 </sst>
 </file>
@@ -1893,12 +1941,12 @@
   <dimension ref="A1:G450"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G153" sqref="G153"/>
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -4712,11 +4760,15 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A150" s="5"/>
+      <c r="A150" s="5" t="s">
+        <v>445</v>
+      </c>
       <c r="B150" s="28" t="s">
         <v>424</v>
       </c>
-      <c r="C150" s="5"/>
+      <c r="C150" s="5" t="s">
+        <v>455</v>
+      </c>
       <c r="D150" s="26">
         <v>7.8</v>
       </c>
@@ -4728,10 +4780,15 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A151" s="5"/>
+      <c r="A151" s="5" t="s">
+        <v>446</v>
+      </c>
       <c r="B151" s="13" t="s">
         <v>425</v>
       </c>
+      <c r="C151" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="D151" s="25">
         <v>18.150000000000002</v>
       </c>
@@ -4743,11 +4800,15 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A152" s="5"/>
+      <c r="A152" s="5" t="s">
+        <v>447</v>
+      </c>
       <c r="B152" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="C152" s="5"/>
+      <c r="C152" s="5" t="s">
+        <v>459</v>
+      </c>
       <c r="D152" s="30">
         <v>23.8</v>
       </c>
@@ -4759,11 +4820,15 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A153" s="5"/>
+      <c r="A153" s="5" t="s">
+        <v>448</v>
+      </c>
       <c r="B153" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="C153" s="5"/>
+      <c r="C153" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="D153" s="32">
         <v>18.22</v>
       </c>
@@ -4775,11 +4840,15 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A154" s="5"/>
+      <c r="A154" s="5" t="s">
+        <v>449</v>
+      </c>
       <c r="B154" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="C154" s="5"/>
+      <c r="C154" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D154" s="35">
         <v>9.82</v>
       </c>
@@ -4791,11 +4860,15 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="5"/>
+      <c r="A155" s="5" t="s">
+        <v>452</v>
+      </c>
       <c r="B155" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C155" s="5"/>
+      <c r="C155" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D155" s="35">
         <v>9.82</v>
       </c>
@@ -4807,11 +4880,15 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="5"/>
+      <c r="A156" s="5" t="s">
+        <v>450</v>
+      </c>
       <c r="B156" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="C156" s="5"/>
+      <c r="C156" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D156" s="35">
         <v>9.82</v>
       </c>
@@ -4823,11 +4900,15 @@
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="5"/>
+      <c r="A157" s="5" t="s">
+        <v>454</v>
+      </c>
       <c r="B157" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="C157" s="5"/>
+      <c r="C157" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D157" s="35">
         <v>9.82</v>
       </c>
@@ -4839,11 +4920,15 @@
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="5"/>
+      <c r="A158" s="5" t="s">
+        <v>451</v>
+      </c>
       <c r="B158" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="C158" s="5"/>
+      <c r="C158" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D158" s="35">
         <v>9.82</v>
       </c>
@@ -4855,11 +4940,15 @@
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="5"/>
+      <c r="A159" s="5" t="s">
+        <v>453</v>
+      </c>
       <c r="B159" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="C159" s="5"/>
+      <c r="C159" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="D159" s="35">
         <v>9.82</v>
       </c>
@@ -4871,11 +4960,15 @@
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="5"/>
+      <c r="A160" s="5" t="s">
+        <v>450</v>
+      </c>
       <c r="B160" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C160" s="5"/>
+      <c r="C160" s="5" t="s">
+        <v>458</v>
+      </c>
       <c r="D160" s="35">
         <v>6.3</v>
       </c>

</xml_diff>